<commit_message>
#288 Finire FF {scrollbehavior: center}
</commit_message>
<xml_diff>
--- a/docs/tp/Sfera_4.0/04.08.22 tp per automatici.xlsx
+++ b/docs/tp/Sfera_4.0/04.08.22 tp per automatici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\matrix-web-fe-tests\docs\tp\Sfera_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D82423-C54E-474F-A134-69A19E41C69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2EA737-1B1B-4C43-AAD1-34FE7BE4496E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3CAC5CA-9857-4B73-8B5C-46816C65856E}"/>
   </bookViews>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F97BA40-992E-4797-82DE-29C97C455A1D}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I17" sqref="A16:I17"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H21" sqref="A12:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,47 +883,60 @@
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="3">
-        <v>2</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="F18" s="6">
+        <v>2</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="330" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="3">
-        <v>2</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="F20" s="6">
+        <v>2</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I20" t="s">
@@ -931,12 +944,18 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>